<commit_message>
debug translate after test
</commit_message>
<xml_diff>
--- a/test/sentence100_test.xlsx
+++ b/test/sentence100_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\thaihmong_translation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD709B9-E100-436B-B28F-A38BAB2ECA95}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737BD71E-CB6C-4013-962E-2CF2F4330BAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>ประโยคทดสอบ</t>
   </si>
@@ -54,9 +54,6 @@
     <t>คำสั่งของฉันคือปล่อยคุณไว้ที่นี่</t>
   </si>
   <si>
-    <t>คุณจะมาที่ที่ทำงานของฉันพรุ่งนี้เช้าได้ไหม</t>
-  </si>
-  <si>
     <t>คุณทราบหรือไม่ว่าการประชุมของคุณเกี่ยวกับเรื่องอะไร</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>ฉันได้รับข้อความของคุณ มีอะไรเหรอ</t>
   </si>
   <si>
-    <t>ฉันต้องการความช่วยเหลือของคุณเดี๋ยวนี้</t>
-  </si>
-  <si>
     <t>ฉันต้องการให้คุณได้พบกับเพื่อนๆ ของฉัน</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>ฉันอยากได้ยินความเห็นของคุณ</t>
   </si>
   <si>
-    <t>ทำตามคำชี้แนะของฉันเป็นอย่างดี</t>
-  </si>
-  <si>
     <t>เธอแก่มากพอที่จะเป็นยายของคุณได้</t>
   </si>
   <si>
@@ -177,9 +168,6 @@
     <t>ใครคือผู้เขียน</t>
   </si>
   <si>
-    <t>มีแอปเปิ้ลบ้างหรือไม่</t>
-  </si>
-  <si>
     <t>สิ่งนี้ เป็นของใคร</t>
   </si>
   <si>
@@ -192,9 +180,6 @@
     <t>ฉันหารถดีๆ คันหนึ่งให้คุณได้แล้ว</t>
   </si>
   <si>
-    <t>ฉันขับรถคันสีฟ้าไปทางาน</t>
-  </si>
-  <si>
     <t>ดีที่ได้พบคุณอีกหลังจากไม่ได้เจอกันนานมาแล้ว</t>
   </si>
   <si>
@@ -222,9 +207,6 @@
     <t>เธอควรจะละอายใจตัวเองนะ</t>
   </si>
   <si>
-    <t>ฉันพาตัวเข้าสู่ปัญหาโดยการ...</t>
-  </si>
-  <si>
     <t>มันเป็นเรื่องส่วนตัว</t>
   </si>
   <si>
@@ -267,9 +249,6 @@
     <t>ฉันไปที่นั่นโดยเครื่องบิน</t>
   </si>
   <si>
-    <t>ฉันพาตัวเข้าสู่ปัญหาโดยการ.</t>
-  </si>
-  <si>
     <t>เธอต้องการให้คุณมาโดยเร็วและอย่าทำให้เธอผิดหวัง</t>
   </si>
   <si>
@@ -285,9 +264,6 @@
     <t>ฉันคิดว่ามันสมบูรณ์แบบโดยแท้จริง</t>
   </si>
   <si>
-    <t>มันควรจะทาโดยนักออกแบบมืออาชีพนะนี่</t>
-  </si>
-  <si>
     <t>มันเหลือเชื่อโดยแท้</t>
   </si>
   <si>
@@ -321,12 +297,6 @@
     <t>ฉันจะไม่ไปจากที่นี่โดยไม่ได้งาน</t>
   </si>
   <si>
-    <t>มีงานสองสามอย่างโดยรอบบ้านที่ฉันอยากให้คุณทา</t>
-  </si>
-  <si>
-    <t>พวกเราควรจะทาสิ่งนั้นโดยทันที</t>
-  </si>
-  <si>
     <t>ก็คิดถึงบ้างบางครั้ง โดยเฉพาะในวันแรกๆ</t>
   </si>
   <si>
@@ -337,13 +307,49 @@
   </si>
   <si>
     <t>ฉันกำลังจะคว้าโอกาสโดยปราศจากความกลัว</t>
+  </si>
+  <si>
+    <t>เขาประทับใจกับงานของคุณมาก</t>
+  </si>
+  <si>
+    <t>คุณจะมาที่ทำงานของฉันวันพรุ่งนี้เช้าได้ไหม</t>
+  </si>
+  <si>
+    <t>ฉันต้องการความช่วยเหลือจากคุณเดี๋ยวนี้</t>
+  </si>
+  <si>
+    <t>ทำตามคำชี้แนะของฉันได้เป็นอย่างดี</t>
+  </si>
+  <si>
+    <t>มีแอปเปิ้ลบ้างไหม</t>
+  </si>
+  <si>
+    <t>ฉันขับรถคันสีฟ้าไปทำงาน</t>
+  </si>
+  <si>
+    <t>ตัวปัญหาคืออะไร</t>
+  </si>
+  <si>
+    <t>ฉันแก้ปัญหาโดยการวิ่ง</t>
+  </si>
+  <si>
+    <t>มันถูกออกแบบโดยนักออกแบบมืออาชีพ</t>
+  </si>
+  <si>
+    <t>ฉันต้องการพูดกับเขาโดยผ่านคุณ</t>
+  </si>
+  <si>
+    <t>คุณต้องทำโดยไม่มีผู้ช่วย</t>
+  </si>
+  <si>
+    <t>พวกเราควรจะทำสิ่งนั้นโดยทันที</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,17 +364,6 @@
     </font>
     <font>
       <sz val="20"/>
-      <color theme="1"/>
-      <name val="TH Niramit AS"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF050505"/>
-      <name val="TH Niramit AS"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color rgb="FF5D5D5D"/>
       <name val="TH Niramit AS"/>
     </font>
   </fonts>
@@ -438,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -448,15 +443,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -761,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.75"/>
@@ -780,12 +777,12 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="3" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -793,7 +790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="4" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -801,7 +798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="5" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -809,15 +806,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="6" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -825,7 +822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="8" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -833,7 +830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="9" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -841,766 +838,766 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+    <row r="10" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30.6" x14ac:dyDescent="0.9">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
-      <c r="B28" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B28" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>1</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B29" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>2</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B30" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>3</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B31" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>4</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B32" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>5</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B33" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>6</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B34" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>7</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B35" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>8</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B36" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>9</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B37" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>10</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B38" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>11</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B39" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>12</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B40" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>13</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B41" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>14</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B42" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>15</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B43" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>16</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B44" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>17</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B45" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>18</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B46" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>19</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B47" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>20</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B48" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>21</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B49" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>22</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B50" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>23</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B51" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>24</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B52" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>25</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>51</v>
+      <c r="B53" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
-      <c r="B54" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B54" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>1</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>2</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>3</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>4</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>5</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>6</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>7</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B61" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>8</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>9</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B63" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>10</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B64" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>11</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>12</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>13</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>14</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>15</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>16</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>17</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>18</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>19</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>20</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>21</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>22</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>23</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>24</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>25</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
-      <c r="B80" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B80" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>1</v>
       </c>
-      <c r="B81" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B81" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>2</v>
       </c>
-      <c r="B82" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B82" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>3</v>
       </c>
-      <c r="B83" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B83" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>4</v>
       </c>
-      <c r="B84" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+      <c r="B84" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>5</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>6</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>7</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>8</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>9</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>10</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>11</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>12</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>13</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>14</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>15</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>16</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>17</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>18</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>19</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>20</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>21</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>22</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>23</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>24</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="30.6" x14ac:dyDescent="0.9">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>25</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>